<commit_message>
DateRange ts and js files
the DateRange code asks the user to enter two dates, and returns the TSA flying stats for the dates in between and including the entered range.
</commit_message>
<xml_diff>
--- a/tsaTableUpdated2.xlsx
+++ b/tsaTableUpdated2.xlsx
@@ -382,2202 +382,2202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>12/22/2020</v>
+        <v>12/23/2020</v>
       </c>
       <c r="B1" t="str">
-        <v>992,167</v>
+        <v>1,191,123</v>
       </c>
       <c r="C1" t="str">
-        <v>1,981,433</v>
+        <v>1,937,235</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>12/21/2020</v>
+        <v>12/22/2020</v>
       </c>
       <c r="B2" t="str">
-        <v>954,782</v>
+        <v>992,167</v>
       </c>
       <c r="C2" t="str">
-        <v>2,490,503</v>
+        <v>1,981,433</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>12/20/2020</v>
+        <v>12/21/2020</v>
       </c>
       <c r="B3" t="str">
-        <v>1,064,619</v>
+        <v>954,782</v>
       </c>
       <c r="C3" t="str">
-        <v>2,519,399</v>
+        <v>2,490,503</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>12/19/2020</v>
+        <v>12/20/2020</v>
       </c>
       <c r="B4" t="str">
-        <v>1,073,563</v>
+        <v>1,064,619</v>
       </c>
       <c r="C4" t="str">
-        <v>2,487,987</v>
+        <v>2,519,399</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>12/18/2020</v>
+        <v>12/19/2020</v>
       </c>
       <c r="B5" t="str">
-        <v>1,066,747</v>
+        <v>1,073,563</v>
       </c>
       <c r="C5" t="str">
-        <v>2,608,088</v>
+        <v>2,487,987</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>12/17/2020</v>
+        <v>12/18/2020</v>
       </c>
       <c r="B6" t="str">
-        <v>846,934</v>
+        <v>1,066,747</v>
       </c>
       <c r="C6" t="str">
-        <v>2,471,408</v>
+        <v>2,608,088</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>12/16/2020</v>
+        <v>12/17/2020</v>
       </c>
       <c r="B7" t="str">
-        <v>641,966</v>
+        <v>846,934</v>
       </c>
       <c r="C7" t="str">
-        <v>2,234,374</v>
+        <v>2,471,408</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>12/15/2020</v>
+        <v>12/16/2020</v>
       </c>
       <c r="B8" t="str">
-        <v>552,024</v>
+        <v>641,966</v>
       </c>
       <c r="C8" t="str">
-        <v>2,009,112</v>
+        <v>2,234,374</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>12/14/2020</v>
+        <v>12/15/2020</v>
       </c>
       <c r="B9" t="str">
-        <v>752,451</v>
+        <v>552,024</v>
       </c>
       <c r="C9" t="str">
-        <v>2,250,386</v>
+        <v>2,009,112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>12/13/2020</v>
+        <v>12/14/2020</v>
       </c>
       <c r="B10" t="str">
-        <v>865,014</v>
+        <v>752,451</v>
       </c>
       <c r="C10" t="str">
-        <v>2,300,248</v>
+        <v>2,250,386</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>12/12/2020</v>
+        <v>12/13/2020</v>
       </c>
       <c r="B11" t="str">
-        <v>662,380</v>
+        <v>865,014</v>
       </c>
       <c r="C11" t="str">
-        <v>1,893,871</v>
+        <v>2,300,248</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>12/11/2020</v>
+        <v>12/12/2020</v>
       </c>
       <c r="B12" t="str">
-        <v>787,489</v>
+        <v>662,380</v>
       </c>
       <c r="C12" t="str">
-        <v>2,388,029</v>
+        <v>1,893,871</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>12/10/2020</v>
+        <v>12/11/2020</v>
       </c>
       <c r="B13" t="str">
-        <v>754,307</v>
+        <v>787,489</v>
       </c>
       <c r="C13" t="str">
-        <v>2,362,310</v>
+        <v>2,388,029</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>12/9/2020</v>
+        <v>12/10/2020</v>
       </c>
       <c r="B14" t="str">
-        <v>564,372</v>
+        <v>754,307</v>
       </c>
       <c r="C14" t="str">
-        <v>2,020,488</v>
+        <v>2,362,310</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>12/8/2020</v>
+        <v>12/9/2020</v>
       </c>
       <c r="B15" t="str">
-        <v>501,513</v>
+        <v>564,372</v>
       </c>
       <c r="C15" t="str">
-        <v>1,897,051</v>
+        <v>2,020,488</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>12/7/2020</v>
+        <v>12/8/2020</v>
       </c>
       <c r="B16" t="str">
-        <v>703,546</v>
+        <v>501,513</v>
       </c>
       <c r="C16" t="str">
-        <v>2,226,290</v>
+        <v>1,897,051</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>12/6/2020</v>
+        <v>12/7/2020</v>
       </c>
       <c r="B17" t="str">
-        <v>837,137</v>
+        <v>703,546</v>
       </c>
       <c r="C17" t="str">
-        <v>2,292,079</v>
+        <v>2,226,290</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>12/5/2020</v>
+        <v>12/6/2020</v>
       </c>
       <c r="B18" t="str">
-        <v>629,430</v>
+        <v>837,137</v>
       </c>
       <c r="C18" t="str">
-        <v>1,755,801</v>
+        <v>2,292,079</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>12/4/2020</v>
+        <v>12/5/2020</v>
       </c>
       <c r="B19" t="str">
-        <v>753,951</v>
+        <v>629,430</v>
       </c>
       <c r="C19" t="str">
-        <v>2,278,205</v>
+        <v>1,755,801</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>12/3/2020</v>
+        <v>12/4/2020</v>
       </c>
       <c r="B20" t="str">
-        <v>738,050</v>
+        <v>753,951</v>
       </c>
       <c r="C20" t="str">
-        <v>2,262,878</v>
+        <v>2,278,205</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>12/2/2020</v>
+        <v>12/3/2020</v>
       </c>
       <c r="B21" t="str">
-        <v>632,356</v>
+        <v>738,050</v>
       </c>
       <c r="C21" t="str">
-        <v>2,054,380</v>
+        <v>2,262,878</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>12/1/2020</v>
+        <v>12/2/2020</v>
       </c>
       <c r="B22" t="str">
-        <v>780,283</v>
+        <v>632,356</v>
       </c>
       <c r="C22" t="str">
-        <v>2,280,403</v>
+        <v>2,054,380</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>11/30/2020</v>
+        <v>12/1/2020</v>
       </c>
       <c r="B23" t="str">
-        <v>981,912</v>
+        <v>780,283</v>
       </c>
       <c r="C23" t="str">
-        <v>2,591,470</v>
+        <v>2,280,403</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>11/29/2020</v>
+        <v>11/30/2020</v>
       </c>
       <c r="B24" t="str">
-        <v>1,176,091</v>
+        <v>981,912</v>
       </c>
       <c r="C24" t="str">
-        <v>2,882,915</v>
+        <v>2,591,470</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>11/28/2020</v>
+        <v>11/29/2020</v>
       </c>
       <c r="B25" t="str">
-        <v>964,630</v>
+        <v>1,176,091</v>
       </c>
       <c r="C25" t="str">
-        <v>2,648,268</v>
+        <v>2,882,915</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>11/27/2020</v>
+        <v>11/28/2020</v>
       </c>
       <c r="B26" t="str">
-        <v>820,399</v>
+        <v>964,630</v>
       </c>
       <c r="C26" t="str">
-        <v>1,968,137</v>
+        <v>2,648,268</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>11/26/2020</v>
+        <v>11/27/2020</v>
       </c>
       <c r="B27" t="str">
-        <v>560,902</v>
+        <v>820,399</v>
       </c>
       <c r="C27" t="str">
-        <v>1,591,158</v>
+        <v>1,968,137</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>11/25/2020</v>
+        <v>11/26/2020</v>
       </c>
       <c r="B28" t="str">
-        <v>1,070,967</v>
+        <v>560,902</v>
       </c>
       <c r="C28" t="str">
-        <v>2,624,250</v>
+        <v>1,591,158</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>11/24/2020</v>
+        <v>11/25/2020</v>
       </c>
       <c r="B29" t="str">
-        <v>912,090</v>
+        <v>1,070,967</v>
       </c>
       <c r="C29" t="str">
-        <v>2,435,170</v>
+        <v>2,624,250</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>11/23/2020</v>
+        <v>11/24/2020</v>
       </c>
       <c r="B30" t="str">
-        <v>917,354</v>
+        <v>912,090</v>
       </c>
       <c r="C30" t="str">
-        <v>2,254,188</v>
+        <v>2,435,170</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>11/22/2020</v>
+        <v>11/23/2020</v>
       </c>
       <c r="B31" t="str">
-        <v>1,047,934</v>
+        <v>917,354</v>
       </c>
       <c r="C31" t="str">
-        <v>2,321,546</v>
+        <v>2,254,188</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>11/21/2020</v>
+        <v>11/22/2020</v>
       </c>
       <c r="B32" t="str">
-        <v>984,369</v>
+        <v>1,047,934</v>
       </c>
       <c r="C32" t="str">
-        <v>2,194,291</v>
+        <v>2,321,546</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>11/20/2020</v>
+        <v>11/21/2020</v>
       </c>
       <c r="B33" t="str">
-        <v>1,019,836</v>
+        <v>984,369</v>
       </c>
       <c r="C33" t="str">
-        <v>2,550,459</v>
+        <v>2,194,291</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>11/19/2020</v>
+        <v>11/20/2020</v>
       </c>
       <c r="B34" t="str">
-        <v>907,332</v>
+        <v>1,019,836</v>
       </c>
       <c r="C34" t="str">
-        <v>2,428,095</v>
+        <v>2,550,459</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>11/18/2020</v>
+        <v>11/19/2020</v>
       </c>
       <c r="B35" t="str">
-        <v>703,135</v>
+        <v>907,332</v>
       </c>
       <c r="C35" t="str">
-        <v>2,071,631</v>
+        <v>2,428,095</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>11/17/2020</v>
+        <v>11/18/2020</v>
       </c>
       <c r="B36" t="str">
-        <v>611,497</v>
+        <v>703,135</v>
       </c>
       <c r="C36" t="str">
-        <v>1,900,895</v>
+        <v>2,071,631</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>11/16/2020</v>
+        <v>11/17/2020</v>
       </c>
       <c r="B37" t="str">
-        <v>883,157</v>
+        <v>611,497</v>
       </c>
       <c r="C37" t="str">
-        <v>2,298,856</v>
+        <v>1,900,895</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>11/15/2020</v>
+        <v>11/16/2020</v>
       </c>
       <c r="B38" t="str">
-        <v>978,297</v>
+        <v>883,157</v>
       </c>
       <c r="C38" t="str">
-        <v>2,396,681</v>
+        <v>2,298,856</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>11/14/2020</v>
+        <v>11/15/2020</v>
       </c>
       <c r="B39" t="str">
-        <v>697,360</v>
+        <v>978,297</v>
       </c>
       <c r="C39" t="str">
-        <v>1,807,230</v>
+        <v>2,396,681</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>11/13/2020</v>
+        <v>11/14/2020</v>
       </c>
       <c r="B40" t="str">
-        <v>881,579</v>
+        <v>697,360</v>
       </c>
       <c r="C40" t="str">
-        <v>2,437,211</v>
+        <v>1,807,230</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>11/12/2020</v>
+        <v>11/13/2020</v>
       </c>
       <c r="B41" t="str">
-        <v>866,679</v>
+        <v>881,579</v>
       </c>
       <c r="C41" t="str">
-        <v>2,364,920</v>
+        <v>2,437,211</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>11/11/2020</v>
+        <v>11/12/2020</v>
       </c>
       <c r="B42" t="str">
-        <v>674,633</v>
+        <v>866,679</v>
       </c>
       <c r="C42" t="str">
-        <v>2,072,207</v>
+        <v>2,364,920</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>11/10/2020</v>
+        <v>11/11/2020</v>
       </c>
       <c r="B43" t="str">
-        <v>596,475</v>
+        <v>674,633</v>
       </c>
       <c r="C43" t="str">
-        <v>2,150,003</v>
+        <v>2,072,207</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>11/9/2020</v>
+        <v>11/10/2020</v>
       </c>
       <c r="B44" t="str">
-        <v>836,600</v>
+        <v>596,475</v>
       </c>
       <c r="C44" t="str">
-        <v>2,465,392</v>
+        <v>2,150,003</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>11/8/2020</v>
+        <v>11/9/2020</v>
       </c>
       <c r="B45" t="str">
-        <v>973,020</v>
+        <v>836,600</v>
       </c>
       <c r="C45" t="str">
-        <v>2,356,349</v>
+        <v>2,465,392</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>11/7/2020</v>
+        <v>11/8/2020</v>
       </c>
       <c r="B46" t="str">
-        <v>689,951</v>
+        <v>973,020</v>
       </c>
       <c r="C46" t="str">
-        <v>1,908,805</v>
+        <v>2,356,349</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>11/6/2020</v>
+        <v>11/7/2020</v>
       </c>
       <c r="B47" t="str">
-        <v>895,091</v>
+        <v>689,951</v>
       </c>
       <c r="C47" t="str">
-        <v>2,544,350</v>
+        <v>1,908,805</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>11/5/2020</v>
+        <v>11/6/2020</v>
       </c>
       <c r="B48" t="str">
-        <v>867,105</v>
+        <v>895,091</v>
       </c>
       <c r="C48" t="str">
-        <v>2,507,365</v>
+        <v>2,544,350</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>11/4/2020</v>
+        <v>11/5/2020</v>
       </c>
       <c r="B49" t="str">
-        <v>636,533</v>
+        <v>867,105</v>
       </c>
       <c r="C49" t="str">
-        <v>2,147,882</v>
+        <v>2,507,365</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>11/3/2020</v>
+        <v>11/4/2020</v>
       </c>
       <c r="B50" t="str">
-        <v>575,829</v>
+        <v>636,533</v>
       </c>
       <c r="C50" t="str">
-        <v>2,005,101</v>
+        <v>2,147,882</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>11/2/2020</v>
+        <v>11/3/2020</v>
       </c>
       <c r="B51" t="str">
-        <v>846,138</v>
+        <v>575,829</v>
       </c>
       <c r="C51" t="str">
-        <v>2,403,304</v>
+        <v>2,005,101</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>11/1/2020</v>
+        <v>11/2/2020</v>
       </c>
       <c r="B52" t="str">
-        <v>936,092</v>
+        <v>846,138</v>
       </c>
       <c r="C52" t="str">
-        <v>2,459,525</v>
+        <v>2,403,304</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>10/31/2020</v>
+        <v>11/1/2020</v>
       </c>
       <c r="B53" t="str">
-        <v>618,476</v>
+        <v>936,092</v>
       </c>
       <c r="C53" t="str">
-        <v>1,836,781</v>
+        <v>2,459,525</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>10/30/2020</v>
+        <v>10/31/2020</v>
       </c>
       <c r="B54" t="str">
-        <v>892,712</v>
+        <v>618,476</v>
       </c>
       <c r="C54" t="str">
-        <v>2,319,906</v>
+        <v>1,836,781</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>10/29/2020</v>
+        <v>10/30/2020</v>
       </c>
       <c r="B55" t="str">
-        <v>873,636</v>
+        <v>892,712</v>
       </c>
       <c r="C55" t="str">
-        <v>2,047,910</v>
+        <v>2,319,906</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>10/28/2020</v>
+        <v>10/29/2020</v>
       </c>
       <c r="B56" t="str">
-        <v>666,957</v>
+        <v>873,636</v>
       </c>
       <c r="C56" t="str">
-        <v>2,066,516</v>
+        <v>2,047,910</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>10/27/2020</v>
+        <v>10/28/2020</v>
       </c>
       <c r="B57" t="str">
-        <v>648,517</v>
+        <v>666,957</v>
       </c>
       <c r="C57" t="str">
-        <v>1,910,506</v>
+        <v>2,066,516</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>10/26/2020</v>
+        <v>10/27/2020</v>
       </c>
       <c r="B58" t="str">
-        <v>898,735</v>
+        <v>648,517</v>
       </c>
       <c r="C58" t="str">
-        <v>2,347,017</v>
+        <v>1,910,506</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>10/25/2020</v>
+        <v>10/26/2020</v>
       </c>
       <c r="B59" t="str">
-        <v>983,745</v>
+        <v>898,735</v>
       </c>
       <c r="C59" t="str">
-        <v>2,478,287</v>
+        <v>2,347,017</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>10/24/2020</v>
+        <v>10/25/2020</v>
       </c>
       <c r="B60" t="str">
-        <v>755,287</v>
+        <v>983,745</v>
       </c>
       <c r="C60" t="str">
-        <v>1,931,971</v>
+        <v>2,478,287</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>10/23/2020</v>
+        <v>10/24/2020</v>
       </c>
       <c r="B61" t="str">
-        <v>958,437</v>
+        <v>755,287</v>
       </c>
       <c r="C61" t="str">
-        <v>2,594,337</v>
+        <v>1,931,971</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>10/22/2020</v>
+        <v>10/23/2020</v>
       </c>
       <c r="B62" t="str">
-        <v>934,386</v>
+        <v>958,437</v>
       </c>
       <c r="C62" t="str">
-        <v>2,541,581</v>
+        <v>2,594,337</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>10/21/2020</v>
+        <v>10/22/2020</v>
       </c>
       <c r="B63" t="str">
-        <v>694,150</v>
+        <v>934,386</v>
       </c>
       <c r="C63" t="str">
-        <v>2,245,199</v>
+        <v>2,541,581</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>10/20/2020</v>
+        <v>10/21/2020</v>
       </c>
       <c r="B64" t="str">
-        <v>662,484</v>
+        <v>694,150</v>
       </c>
       <c r="C64" t="str">
-        <v>2,126,637</v>
+        <v>2,245,199</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>10/19/2020</v>
+        <v>10/20/2020</v>
       </c>
       <c r="B65" t="str">
-        <v>921,031</v>
+        <v>662,484</v>
       </c>
       <c r="C65" t="str">
-        <v>2,514,673</v>
+        <v>2,126,637</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>10/18/2020</v>
+        <v>10/19/2020</v>
       </c>
       <c r="B66" t="str">
-        <v>1,031,505</v>
+        <v>921,031</v>
       </c>
       <c r="C66" t="str">
-        <v>2,606,266</v>
+        <v>2,514,673</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>10/17/2020</v>
+        <v>10/18/2020</v>
       </c>
       <c r="B67" t="str">
-        <v>788,743</v>
+        <v>1,031,505</v>
       </c>
       <c r="C67" t="str">
-        <v>2,049,855</v>
+        <v>2,606,266</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>10/16/2020</v>
+        <v>10/17/2020</v>
       </c>
       <c r="B68" t="str">
-        <v>973,046</v>
+        <v>788,743</v>
       </c>
       <c r="C68" t="str">
-        <v>2,637,667</v>
+        <v>2,049,855</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>10/15/2020</v>
+        <v>10/16/2020</v>
       </c>
       <c r="B69" t="str">
-        <v>950,024</v>
+        <v>973,046</v>
       </c>
       <c r="C69" t="str">
-        <v>2,581,007</v>
+        <v>2,637,667</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>10/14/2020</v>
+        <v>10/15/2020</v>
       </c>
       <c r="B70" t="str">
-        <v>717,940</v>
+        <v>950,024</v>
       </c>
       <c r="C70" t="str">
-        <v>2,317,763</v>
+        <v>2,581,007</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>10/13/2020</v>
+        <v>10/14/2020</v>
       </c>
       <c r="B71" t="str">
-        <v>680,894</v>
+        <v>717,940</v>
       </c>
       <c r="C71" t="str">
-        <v>2,313,632</v>
+        <v>2,317,763</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>10/12/2020</v>
+        <v>10/13/2020</v>
       </c>
       <c r="B72" t="str">
-        <v>958,440</v>
+        <v>680,894</v>
       </c>
       <c r="C72" t="str">
-        <v>2,616,771</v>
+        <v>2,313,632</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>10/11/2020</v>
+        <v>10/12/2020</v>
       </c>
       <c r="B73" t="str">
-        <v>984,234</v>
+        <v>958,440</v>
       </c>
       <c r="C73" t="str">
-        <v>2,555,333</v>
+        <v>2,616,771</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>10/10/2020</v>
+        <v>10/11/2020</v>
       </c>
       <c r="B74" t="str">
-        <v>769,868</v>
+        <v>984,234</v>
       </c>
       <c r="C74" t="str">
-        <v>2,074,718</v>
+        <v>2,555,333</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>10/9/2020</v>
+        <v>10/10/2020</v>
       </c>
       <c r="B75" t="str">
-        <v>968,545</v>
+        <v>769,868</v>
       </c>
       <c r="C75" t="str">
-        <v>2,688,032</v>
+        <v>2,074,718</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>10/8/2020</v>
+        <v>10/9/2020</v>
       </c>
       <c r="B76" t="str">
-        <v>936,915</v>
+        <v>968,545</v>
       </c>
       <c r="C76" t="str">
-        <v>2,605,291</v>
+        <v>2,688,032</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>10/7/2020</v>
+        <v>10/8/2020</v>
       </c>
       <c r="B77" t="str">
-        <v>668,519</v>
+        <v>936,915</v>
       </c>
       <c r="C77" t="str">
-        <v>2,215,233</v>
+        <v>2,605,291</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>10/6/2020</v>
+        <v>10/7/2020</v>
       </c>
       <c r="B78" t="str">
-        <v>590,766</v>
+        <v>668,519</v>
       </c>
       <c r="C78" t="str">
-        <v>2,035,628</v>
+        <v>2,215,233</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>10/5/2020</v>
+        <v>10/6/2020</v>
       </c>
       <c r="B79" t="str">
-        <v>816,838</v>
+        <v>590,766</v>
       </c>
       <c r="C79" t="str">
-        <v>2,400,153</v>
+        <v>2,035,628</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>10/4/2020</v>
+        <v>10/5/2020</v>
       </c>
       <c r="B80" t="str">
-        <v>900,911</v>
+        <v>816,838</v>
       </c>
       <c r="C80" t="str">
-        <v>2,542,118</v>
+        <v>2,400,153</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>10/3/2020</v>
+        <v>10/4/2020</v>
       </c>
       <c r="B81" t="str">
-        <v>677,661</v>
+        <v>900,911</v>
       </c>
       <c r="C81" t="str">
-        <v>1,921,185</v>
+        <v>2,542,118</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>10/2/2020</v>
+        <v>10/3/2020</v>
       </c>
       <c r="B82" t="str">
-        <v>857,186</v>
+        <v>677,661</v>
       </c>
       <c r="C82" t="str">
-        <v>2,526,835</v>
+        <v>1,921,185</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>10/1/2020</v>
+        <v>10/2/2020</v>
       </c>
       <c r="B83" t="str">
-        <v>855,908</v>
+        <v>857,186</v>
       </c>
       <c r="C83" t="str">
-        <v>2,447,687</v>
+        <v>2,526,835</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>9/30/2020</v>
+        <v>10/1/2020</v>
       </c>
       <c r="B84" t="str">
-        <v>634,046</v>
+        <v>855,908</v>
       </c>
       <c r="C84" t="str">
-        <v>2,082,179</v>
+        <v>2,447,687</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>9/29/2020</v>
+        <v>9/30/2020</v>
       </c>
       <c r="B85" t="str">
-        <v>568,688</v>
+        <v>634,046</v>
       </c>
       <c r="C85" t="str">
-        <v>1,998,980</v>
+        <v>2,082,179</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>9/28/2020</v>
+        <v>9/29/2020</v>
       </c>
       <c r="B86" t="str">
-        <v>797,699</v>
+        <v>568,688</v>
       </c>
       <c r="C86" t="str">
-        <v>2,368,818</v>
+        <v>1,998,980</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>9/27/2020</v>
+        <v>9/28/2020</v>
       </c>
       <c r="B87" t="str">
-        <v>873,038</v>
+        <v>797,699</v>
       </c>
       <c r="C87" t="str">
-        <v>2,452,596</v>
+        <v>2,368,818</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>9/26/2020</v>
+        <v>9/27/2020</v>
       </c>
       <c r="B88" t="str">
-        <v>659,350</v>
+        <v>873,038</v>
       </c>
       <c r="C88" t="str">
-        <v>1,966,234</v>
+        <v>2,452,596</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>9/25/2020</v>
+        <v>9/26/2020</v>
       </c>
       <c r="B89" t="str">
-        <v>826,329</v>
+        <v>659,350</v>
       </c>
       <c r="C89" t="str">
-        <v>2,547,611</v>
+        <v>1,966,234</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>9/24/2020</v>
+        <v>9/25/2020</v>
       </c>
       <c r="B90" t="str">
-        <v>826,316</v>
+        <v>826,329</v>
       </c>
       <c r="C90" t="str">
-        <v>2,510,926</v>
+        <v>2,547,611</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>9/23/2020</v>
+        <v>9/24/2020</v>
       </c>
       <c r="B91" t="str">
-        <v>608,726</v>
+        <v>826,316</v>
       </c>
       <c r="C91" t="str">
-        <v>2,188,236</v>
+        <v>2,510,926</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>9/22/2020</v>
+        <v>9/23/2020</v>
       </c>
       <c r="B92" t="str">
-        <v>549,741</v>
+        <v>608,726</v>
       </c>
       <c r="C92" t="str">
-        <v>2,033,490</v>
+        <v>2,188,236</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>9/21/2020</v>
+        <v>9/22/2020</v>
       </c>
       <c r="B93" t="str">
-        <v>769,936</v>
+        <v>549,741</v>
       </c>
       <c r="C93" t="str">
-        <v>2,431,388</v>
+        <v>2,033,490</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>9/20/2020</v>
+        <v>9/21/2020</v>
       </c>
       <c r="B94" t="str">
-        <v>847,968</v>
+        <v>769,936</v>
       </c>
       <c r="C94" t="str">
-        <v>2,517,826</v>
+        <v>2,431,388</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>9/19/2020</v>
+        <v>9/20/2020</v>
       </c>
       <c r="B95" t="str">
-        <v>638,575</v>
+        <v>847,968</v>
       </c>
       <c r="C95" t="str">
-        <v>1,938,402</v>
+        <v>2,517,826</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>9/18/2020</v>
+        <v>9/19/2020</v>
       </c>
       <c r="B96" t="str">
-        <v>812,214</v>
+        <v>638,575</v>
       </c>
       <c r="C96" t="str">
-        <v>2,571,924</v>
+        <v>1,938,402</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>9/17/2020</v>
+        <v>9/18/2020</v>
       </c>
       <c r="B97" t="str">
-        <v>784,746</v>
+        <v>812,214</v>
       </c>
       <c r="C97" t="str">
-        <v>2,455,410</v>
+        <v>2,571,924</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>9/16/2020</v>
+        <v>9/17/2020</v>
       </c>
       <c r="B98" t="str">
-        <v>577,847</v>
+        <v>784,746</v>
       </c>
       <c r="C98" t="str">
-        <v>2,146,857</v>
+        <v>2,455,410</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>9/15/2020</v>
+        <v>9/16/2020</v>
       </c>
       <c r="B99" t="str">
-        <v>522,383</v>
+        <v>577,847</v>
       </c>
       <c r="C99" t="str">
-        <v>2,013,050</v>
+        <v>2,146,857</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>9/14/2020</v>
+        <v>9/15/2020</v>
       </c>
       <c r="B100" t="str">
-        <v>729,558</v>
+        <v>522,383</v>
       </c>
       <c r="C100" t="str">
-        <v>2,405,832</v>
+        <v>2,013,050</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>9/13/2020</v>
+        <v>9/14/2020</v>
       </c>
       <c r="B101" t="str">
-        <v>809,850</v>
+        <v>729,558</v>
       </c>
       <c r="C101" t="str">
-        <v>2,485,134</v>
+        <v>2,405,832</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>9/12/2020</v>
+        <v>9/13/2020</v>
       </c>
       <c r="B102" t="str">
-        <v>613,703</v>
+        <v>809,850</v>
       </c>
       <c r="C102" t="str">
-        <v>1,879,822</v>
+        <v>2,485,134</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>9/11/2020</v>
+        <v>9/12/2020</v>
       </c>
       <c r="B103" t="str">
-        <v>731,353</v>
+        <v>613,703</v>
       </c>
       <c r="C103" t="str">
-        <v>2,484,025</v>
+        <v>1,879,822</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>9/10/2020</v>
+        <v>9/11/2020</v>
       </c>
       <c r="B104" t="str">
-        <v>755,051</v>
+        <v>731,353</v>
       </c>
       <c r="C104" t="str">
-        <v>2,449,302</v>
+        <v>2,484,025</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>9/9/2020</v>
+        <v>9/10/2020</v>
       </c>
       <c r="B105" t="str">
-        <v>616,923</v>
+        <v>755,051</v>
       </c>
       <c r="C105" t="str">
-        <v>2,005,867</v>
+        <v>2,449,302</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>9/8/2020</v>
+        <v>9/9/2020</v>
       </c>
       <c r="B106" t="str">
-        <v>704,075</v>
+        <v>616,923</v>
       </c>
       <c r="C106" t="str">
-        <v>1,943,379</v>
+        <v>2,005,867</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>9/7/2020</v>
+        <v>9/8/2020</v>
       </c>
       <c r="B107" t="str">
-        <v>935,308</v>
+        <v>704,075</v>
       </c>
       <c r="C107" t="str">
-        <v>2,292,985</v>
+        <v>1,943,379</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>9/6/2020</v>
+        <v>9/7/2020</v>
       </c>
       <c r="B108" t="str">
-        <v>689,630</v>
+        <v>935,308</v>
       </c>
       <c r="C108" t="str">
-        <v>2,370,003</v>
+        <v>2,292,985</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>9/5/2020</v>
+        <v>9/6/2020</v>
       </c>
       <c r="B109" t="str">
-        <v>664,640</v>
+        <v>689,630</v>
       </c>
       <c r="C109" t="str">
-        <v>1,755,502</v>
+        <v>2,370,003</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>9/4/2020</v>
+        <v>9/5/2020</v>
       </c>
       <c r="B110" t="str">
-        <v>968,673</v>
+        <v>664,640</v>
       </c>
       <c r="C110" t="str">
-        <v>2,198,828</v>
+        <v>1,755,502</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>9/3/2020</v>
+        <v>9/4/2020</v>
       </c>
       <c r="B111" t="str">
-        <v>877,698</v>
+        <v>968,673</v>
       </c>
       <c r="C111" t="str">
-        <v>2,109,858</v>
+        <v>2,198,828</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>9/2/2020</v>
+        <v>9/3/2020</v>
       </c>
       <c r="B112" t="str">
-        <v>578,131</v>
+        <v>877,698</v>
       </c>
       <c r="C112" t="str">
-        <v>1,889,044</v>
+        <v>2,109,858</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>9/1/2020</v>
+        <v>9/2/2020</v>
       </c>
       <c r="B113" t="str">
-        <v>516,068</v>
+        <v>578,131</v>
       </c>
       <c r="C113" t="str">
-        <v>2,037,750</v>
+        <v>1,889,044</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>8/31/2020</v>
+        <v>9/1/2020</v>
       </c>
       <c r="B114" t="str">
-        <v>711,178</v>
+        <v>516,068</v>
       </c>
       <c r="C114" t="str">
-        <v>2,278,159</v>
+        <v>2,037,750</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>8/30/2020</v>
+        <v>8/31/2020</v>
       </c>
       <c r="B115" t="str">
-        <v>807,695</v>
+        <v>711,178</v>
       </c>
       <c r="C115" t="str">
-        <v>1,887,845</v>
+        <v>2,278,159</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>8/29/2020</v>
+        <v>8/30/2020</v>
       </c>
       <c r="B116" t="str">
-        <v>591,734</v>
+        <v>807,695</v>
       </c>
       <c r="C116" t="str">
-        <v>1,954,902</v>
+        <v>1,887,845</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>8/28/2020</v>
+        <v>8/29/2020</v>
       </c>
       <c r="B117" t="str">
-        <v>738,873</v>
+        <v>591,734</v>
       </c>
       <c r="C117" t="str">
-        <v>2,658,558</v>
+        <v>1,954,902</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>8/27/2020</v>
+        <v>8/28/2020</v>
       </c>
       <c r="B118" t="str">
-        <v>721,060</v>
+        <v>738,873</v>
       </c>
       <c r="C118" t="str">
-        <v>2,561,109</v>
+        <v>2,658,558</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>8/26/2020</v>
+        <v>8/27/2020</v>
       </c>
       <c r="B119" t="str">
-        <v>540,043</v>
+        <v>721,060</v>
       </c>
       <c r="C119" t="str">
-        <v>2,188,688</v>
+        <v>2,561,109</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>8/25/2020</v>
+        <v>8/26/2020</v>
       </c>
       <c r="B120" t="str">
-        <v>523,186</v>
+        <v>540,043</v>
       </c>
       <c r="C120" t="str">
-        <v>2,015,088</v>
+        <v>2,188,688</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>8/24/2020</v>
+        <v>8/25/2020</v>
       </c>
       <c r="B121" t="str">
-        <v>726,788</v>
+        <v>523,186</v>
       </c>
       <c r="C121" t="str">
-        <v>2,358,007</v>
+        <v>2,015,088</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>8/23/2020</v>
+        <v>8/24/2020</v>
       </c>
       <c r="B122" t="str">
-        <v>841,806</v>
+        <v>726,788</v>
       </c>
       <c r="C122" t="str">
-        <v>2,493,162</v>
+        <v>2,358,007</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>8/22/2020</v>
+        <v>8/23/2020</v>
       </c>
       <c r="B123" t="str">
-        <v>625,822</v>
+        <v>841,806</v>
       </c>
       <c r="C123" t="str">
-        <v>2,039,233</v>
+        <v>2,493,162</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>8/21/2020</v>
+        <v>8/22/2020</v>
       </c>
       <c r="B124" t="str">
-        <v>764,468</v>
+        <v>625,822</v>
       </c>
       <c r="C124" t="str">
-        <v>2,559,244</v>
+        <v>2,039,233</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>8/20/2020</v>
+        <v>8/21/2020</v>
       </c>
       <c r="B125" t="str">
-        <v>772,380</v>
+        <v>764,468</v>
       </c>
       <c r="C125" t="str">
-        <v>2,533,184</v>
+        <v>2,559,244</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>8/19/2020</v>
+        <v>8/20/2020</v>
       </c>
       <c r="B126" t="str">
-        <v>586,718</v>
+        <v>772,380</v>
       </c>
       <c r="C126" t="str">
-        <v>2,306,838</v>
+        <v>2,533,184</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>8/18/2020</v>
+        <v>8/19/2020</v>
       </c>
       <c r="B127" t="str">
-        <v>565,946</v>
+        <v>586,718</v>
       </c>
       <c r="C127" t="str">
-        <v>2,247,446</v>
+        <v>2,306,838</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>8/17/2020</v>
+        <v>8/18/2020</v>
       </c>
       <c r="B128" t="str">
-        <v>773,319</v>
+        <v>565,946</v>
       </c>
       <c r="C128" t="str">
-        <v>2,576,965</v>
+        <v>2,247,446</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>8/16/2020</v>
+        <v>8/17/2020</v>
       </c>
       <c r="B129" t="str">
-        <v>862,949</v>
+        <v>773,319</v>
       </c>
       <c r="C129" t="str">
-        <v>2,584,444</v>
+        <v>2,576,965</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>8/15/2020</v>
+        <v>8/16/2020</v>
       </c>
       <c r="B130" t="str">
-        <v>689,895</v>
+        <v>862,949</v>
       </c>
       <c r="C130" t="str">
-        <v>2,171,962</v>
+        <v>2,584,444</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>8/14/2020</v>
+        <v>8/15/2020</v>
       </c>
       <c r="B131" t="str">
-        <v>783,744</v>
+        <v>689,895</v>
       </c>
       <c r="C131" t="str">
-        <v>2,627,564</v>
+        <v>2,171,962</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>8/13/2020</v>
+        <v>8/14/2020</v>
       </c>
       <c r="B132" t="str">
-        <v>761,821</v>
+        <v>783,744</v>
       </c>
       <c r="C132" t="str">
-        <v>2,602,446</v>
+        <v>2,627,564</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>8/12/2020</v>
+        <v>8/13/2020</v>
       </c>
       <c r="B133" t="str">
-        <v>590,749</v>
+        <v>761,821</v>
       </c>
       <c r="C133" t="str">
-        <v>2,391,906</v>
+        <v>2,602,446</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>8/11/2020</v>
+        <v>8/12/2020</v>
       </c>
       <c r="B134" t="str">
-        <v>559,420</v>
+        <v>590,749</v>
       </c>
       <c r="C134" t="str">
-        <v>2,306,829</v>
+        <v>2,391,906</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>8/10/2020</v>
+        <v>8/11/2020</v>
       </c>
       <c r="B135" t="str">
-        <v>761,861</v>
+        <v>559,420</v>
       </c>
       <c r="C135" t="str">
-        <v>2,567,986</v>
+        <v>2,306,829</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>8/9/2020</v>
+        <v>8/10/2020</v>
       </c>
       <c r="B136" t="str">
-        <v>831,789</v>
+        <v>761,861</v>
       </c>
       <c r="C136" t="str">
-        <v>2,647,897</v>
+        <v>2,567,986</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>8/8/2020</v>
+        <v>8/9/2020</v>
       </c>
       <c r="B137" t="str">
-        <v>683,212</v>
+        <v>831,789</v>
       </c>
       <c r="C137" t="str">
-        <v>2,290,340</v>
+        <v>2,647,897</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>8/7/2020</v>
+        <v>8/8/2020</v>
       </c>
       <c r="B138" t="str">
-        <v>762,547</v>
+        <v>683,212</v>
       </c>
       <c r="C138" t="str">
-        <v>2,725,000</v>
+        <v>2,290,340</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>8/6/2020</v>
+        <v>8/7/2020</v>
       </c>
       <c r="B139" t="str">
-        <v>743,599</v>
+        <v>762,547</v>
       </c>
       <c r="C139" t="str">
-        <v>2,707,986</v>
+        <v>2,725,000</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>8/5/2020</v>
+        <v>8/6/2020</v>
       </c>
       <c r="B140" t="str">
-        <v>595,739</v>
+        <v>743,599</v>
       </c>
       <c r="C140" t="str">
-        <v>2,430,094</v>
+        <v>2,707,986</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>8/4/2020</v>
+        <v>8/5/2020</v>
       </c>
       <c r="B141" t="str">
-        <v>543,601</v>
+        <v>595,739</v>
       </c>
       <c r="C141" t="str">
-        <v>2,387,115</v>
+        <v>2,430,094</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>8/3/2020</v>
+        <v>8/4/2020</v>
       </c>
       <c r="B142" t="str">
-        <v>737,235</v>
+        <v>543,601</v>
       </c>
       <c r="C142" t="str">
-        <v>2,619,406</v>
+        <v>2,387,115</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>8/2/2020</v>
+        <v>8/3/2020</v>
       </c>
       <c r="B143" t="str">
-        <v>799,861</v>
+        <v>737,235</v>
       </c>
       <c r="C143" t="str">
-        <v>2,688,640</v>
+        <v>2,619,406</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>8/1/2020</v>
+        <v>8/2/2020</v>
       </c>
       <c r="B144" t="str">
-        <v>709,033</v>
+        <v>799,861</v>
       </c>
       <c r="C144" t="str">
-        <v>2,367,967</v>
+        <v>2,688,640</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>7/31/2020</v>
+        <v>8/1/2020</v>
       </c>
       <c r="B145" t="str">
-        <v>767,320</v>
+        <v>709,033</v>
       </c>
       <c r="C145" t="str">
-        <v>2,730,936</v>
+        <v>2,367,967</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>7/30/2020</v>
+        <v>7/31/2020</v>
       </c>
       <c r="B146" t="str">
-        <v>718,310</v>
+        <v>767,320</v>
       </c>
       <c r="C146" t="str">
-        <v>2,742,882</v>
+        <v>2,730,936</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>7/29/2020</v>
+        <v>7/30/2020</v>
       </c>
       <c r="B147" t="str">
-        <v>573,200</v>
+        <v>718,310</v>
       </c>
       <c r="C147" t="str">
-        <v>2,542,365</v>
+        <v>2,742,882</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>7/28/2020</v>
+        <v>7/29/2020</v>
       </c>
       <c r="B148" t="str">
-        <v>536,756</v>
+        <v>573,200</v>
       </c>
       <c r="C148" t="str">
-        <v>2,438,967</v>
+        <v>2,542,365</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>7/27/2020</v>
+        <v>7/28/2020</v>
       </c>
       <c r="B149" t="str">
-        <v>700,043</v>
+        <v>536,756</v>
       </c>
       <c r="C149" t="str">
-        <v>2,613,346</v>
+        <v>2,438,967</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>7/26/2020</v>
+        <v>7/27/2020</v>
       </c>
       <c r="B150" t="str">
-        <v>751,205</v>
+        <v>700,043</v>
       </c>
       <c r="C150" t="str">
-        <v>2,700,723</v>
+        <v>2,613,346</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>7/25/2020</v>
+        <v>7/26/2020</v>
       </c>
       <c r="B151" t="str">
-        <v>649,027</v>
+        <v>751,205</v>
       </c>
       <c r="C151" t="str">
-        <v>2,364,925</v>
+        <v>2,700,723</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>7/24/2020</v>
+        <v>7/25/2020</v>
       </c>
       <c r="B152" t="str">
-        <v>724,770</v>
+        <v>649,027</v>
       </c>
       <c r="C152" t="str">
-        <v>2,732,770</v>
+        <v>2,364,925</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>7/23/2020</v>
+        <v>7/24/2020</v>
       </c>
       <c r="B153" t="str">
-        <v>704,815</v>
+        <v>724,770</v>
       </c>
       <c r="C153" t="str">
-        <v>2,705,399</v>
+        <v>2,732,770</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>7/22/2020</v>
+        <v>7/23/2020</v>
       </c>
       <c r="B154" t="str">
-        <v>570,951</v>
+        <v>704,815</v>
       </c>
       <c r="C154" t="str">
-        <v>2,561,911</v>
+        <v>2,705,399</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>7/21/2020</v>
+        <v>7/22/2020</v>
       </c>
       <c r="B155" t="str">
-        <v>530,421</v>
+        <v>570,951</v>
       </c>
       <c r="C155" t="str">
-        <v>2,499,460</v>
+        <v>2,561,911</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>7/20/2020</v>
+        <v>7/21/2020</v>
       </c>
       <c r="B156" t="str">
-        <v>695,330</v>
+        <v>530,421</v>
       </c>
       <c r="C156" t="str">
-        <v>2,635,312</v>
+        <v>2,499,460</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>7/19/2020</v>
+        <v>7/20/2020</v>
       </c>
       <c r="B157" t="str">
-        <v>747,422</v>
+        <v>695,330</v>
       </c>
       <c r="C157" t="str">
-        <v>2,727,355</v>
+        <v>2,635,312</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>7/18/2020</v>
+        <v>7/19/2020</v>
       </c>
       <c r="B158" t="str">
-        <v>646,654</v>
+        <v>747,422</v>
       </c>
       <c r="C158" t="str">
-        <v>2,396,462</v>
+        <v>2,727,355</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>7/17/2020</v>
+        <v>7/18/2020</v>
       </c>
       <c r="B159" t="str">
-        <v>720,378</v>
+        <v>646,654</v>
       </c>
       <c r="C159" t="str">
-        <v>2,776,960</v>
+        <v>2,396,462</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>7/16/2020</v>
+        <v>7/17/2020</v>
       </c>
       <c r="B160" t="str">
-        <v>706,164</v>
+        <v>720,378</v>
       </c>
       <c r="C160" t="str">
-        <v>2,716,828</v>
+        <v>2,776,960</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>7/15/2020</v>
+        <v>7/16/2020</v>
       </c>
       <c r="B161" t="str">
-        <v>589,285</v>
+        <v>706,164</v>
       </c>
       <c r="C161" t="str">
-        <v>2,522,563</v>
+        <v>2,716,828</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>7/14/2020</v>
+        <v>7/15/2020</v>
       </c>
       <c r="B162" t="str">
-        <v>540,268</v>
+        <v>589,285</v>
       </c>
       <c r="C162" t="str">
-        <v>2,447,177</v>
+        <v>2,522,563</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>7/13/2020</v>
+        <v>7/14/2020</v>
       </c>
       <c r="B163" t="str">
-        <v>697,985</v>
+        <v>540,268</v>
       </c>
       <c r="C163" t="str">
-        <v>2,615,115</v>
+        <v>2,447,177</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>7/12/2020</v>
+        <v>7/13/2020</v>
       </c>
       <c r="B164" t="str">
-        <v>754,545</v>
+        <v>697,985</v>
       </c>
       <c r="C164" t="str">
-        <v>2,669,717</v>
+        <v>2,615,115</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>7/11/2020</v>
+        <v>7/12/2020</v>
       </c>
       <c r="B165" t="str">
-        <v>656,284</v>
+        <v>754,545</v>
       </c>
       <c r="C165" t="str">
-        <v>2,312,178</v>
+        <v>2,669,717</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>7/10/2020</v>
+        <v>7/11/2020</v>
       </c>
       <c r="B166" t="str">
-        <v>711,124</v>
+        <v>656,284</v>
       </c>
       <c r="C166" t="str">
-        <v>2,716,812</v>
+        <v>2,312,178</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>7/9/2020</v>
+        <v>7/10/2020</v>
       </c>
       <c r="B167" t="str">
-        <v>709,653</v>
+        <v>711,124</v>
       </c>
       <c r="C167" t="str">
-        <v>2,608,209</v>
+        <v>2,716,812</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>7/8/2020</v>
+        <v>7/9/2020</v>
       </c>
       <c r="B168" t="str">
-        <v>632,498</v>
+        <v>709,653</v>
       </c>
       <c r="C168" t="str">
-        <v>2,515,902</v>
+        <v>2,608,209</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>7/7/2020</v>
+        <v>7/8/2020</v>
       </c>
       <c r="B169" t="str">
-        <v>641,761</v>
+        <v>632,498</v>
       </c>
       <c r="C169" t="str">
-        <v>2,506,859</v>
+        <v>2,515,902</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>7/6/2020</v>
+        <v>7/7/2020</v>
       </c>
       <c r="B170" t="str">
-        <v>755,555</v>
+        <v>641,761</v>
       </c>
       <c r="C170" t="str">
-        <v>2,748,718</v>
+        <v>2,506,859</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>7/5/2020</v>
+        <v>7/6/2020</v>
       </c>
       <c r="B171" t="str">
-        <v>732,123</v>
+        <v>755,555</v>
       </c>
       <c r="C171" t="str">
-        <v>2,795,369</v>
+        <v>2,748,718</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>7/4/2020</v>
+        <v>7/5/2020</v>
       </c>
       <c r="B172" t="str">
-        <v>466,669</v>
+        <v>732,123</v>
       </c>
       <c r="C172" t="str">
-        <v>2,345,846</v>
+        <v>2,795,369</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>7/3/2020</v>
+        <v>7/4/2020</v>
       </c>
       <c r="B173" t="str">
-        <v>718,988</v>
+        <v>466,669</v>
       </c>
       <c r="C173" t="str">
-        <v>2,184,253</v>
+        <v>2,345,846</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>7/2/2020</v>
+        <v>7/3/2020</v>
       </c>
       <c r="B174" t="str">
-        <v>764,761</v>
+        <v>718,988</v>
       </c>
       <c r="C174" t="str">
-        <v>2,088,760</v>
+        <v>2,184,253</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>7/1/2020</v>
+        <v>7/2/2020</v>
       </c>
       <c r="B175" t="str">
-        <v>626,516</v>
+        <v>764,761</v>
       </c>
       <c r="C175" t="str">
-        <v>2,547,889</v>
+        <v>2,088,760</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>6/30/2020</v>
+        <v>7/1/2020</v>
       </c>
       <c r="B176" t="str">
-        <v>500,054</v>
+        <v>626,516</v>
       </c>
       <c r="C176" t="str">
-        <v>2,347,767</v>
+        <v>2,547,889</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>6/29/2020</v>
+        <v>6/30/2020</v>
       </c>
       <c r="B177" t="str">
-        <v>625,235</v>
+        <v>500,054</v>
       </c>
       <c r="C177" t="str">
-        <v>2,455,536</v>
+        <v>2,347,767</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>6/28/2020</v>
+        <v>6/29/2020</v>
       </c>
       <c r="B178" t="str">
-        <v>633,810</v>
+        <v>625,235</v>
       </c>
       <c r="C178" t="str">
-        <v>2,632,030</v>
+        <v>2,455,536</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>6/27/2020</v>
+        <v>6/28/2020</v>
       </c>
       <c r="B179" t="str">
-        <v>546,310</v>
+        <v>633,810</v>
       </c>
       <c r="C179" t="str">
-        <v>2,368,846</v>
+        <v>2,632,030</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>6/26/2020</v>
+        <v>6/27/2020</v>
       </c>
       <c r="B180" t="str">
-        <v>632,984</v>
+        <v>546,310</v>
       </c>
       <c r="C180" t="str">
-        <v>2,730,515</v>
+        <v>2,368,846</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>6/25/2020</v>
+        <v>6/26/2020</v>
       </c>
       <c r="B181" t="str">
-        <v>623,624</v>
+        <v>632,984</v>
       </c>
       <c r="C181" t="str">
-        <v>2,711,222</v>
+        <v>2,730,515</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>6/24/2020</v>
+        <v>6/25/2020</v>
       </c>
       <c r="B182" t="str">
-        <v>494,826</v>
+        <v>623,624</v>
       </c>
       <c r="C182" t="str">
-        <v>2,594,661</v>
+        <v>2,711,222</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>6/23/2020</v>
+        <v>6/24/2020</v>
       </c>
       <c r="B183" t="str">
-        <v>471,421</v>
+        <v>494,826</v>
       </c>
       <c r="C183" t="str">
-        <v>2,506,510</v>
+        <v>2,594,661</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>6/22/2020</v>
+        <v>6/23/2020</v>
       </c>
       <c r="B184" t="str">
-        <v>607,540</v>
+        <v>471,421</v>
       </c>
       <c r="C184" t="str">
-        <v>2,716,428</v>
+        <v>2,506,510</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>6/21/2020</v>
+        <v>6/22/2020</v>
       </c>
       <c r="B185" t="str">
-        <v>590,456</v>
+        <v>607,540</v>
       </c>
       <c r="C185" t="str">
-        <v>2,719,643</v>
+        <v>2,716,428</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>6/20/2020</v>
+        <v>6/21/2020</v>
       </c>
       <c r="B186" t="str">
-        <v>507,129</v>
+        <v>590,456</v>
       </c>
       <c r="C186" t="str">
-        <v>2,378,559</v>
+        <v>2,719,643</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>6/19/2020</v>
+        <v>6/20/2020</v>
       </c>
       <c r="B187" t="str">
-        <v>587,908</v>
+        <v>507,129</v>
       </c>
       <c r="C187" t="str">
-        <v>2,772,903</v>
+        <v>2,378,559</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>6/18/2020</v>
+        <v>6/19/2020</v>
       </c>
       <c r="B188" t="str">
-        <v>576,514</v>
+        <v>587,908</v>
       </c>
       <c r="C188" t="str">
-        <v>2,728,786</v>
+        <v>2,772,903</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>6/17/2020</v>
+        <v>6/18/2020</v>
       </c>
       <c r="B189" t="str">
-        <v>441,829</v>
+        <v>576,514</v>
       </c>
       <c r="C189" t="str">
-        <v>2,552,395</v>
+        <v>2,728,786</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>6/16/2020</v>
+        <v>6/17/2020</v>
       </c>
       <c r="B190" t="str">
-        <v>417,924</v>
+        <v>441,829</v>
       </c>
       <c r="C190" t="str">
-        <v>2,466,574</v>
+        <v>2,552,395</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>6/15/2020</v>
+        <v>6/16/2020</v>
       </c>
       <c r="B191" t="str">
-        <v>534,528</v>
+        <v>417,924</v>
       </c>
       <c r="C191" t="str">
-        <v>2,699,580</v>
+        <v>2,466,574</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>6/14/2020</v>
+        <v>6/15/2020</v>
       </c>
       <c r="B192" t="str">
-        <v>544,046</v>
+        <v>534,528</v>
       </c>
       <c r="C192" t="str">
-        <v>2,642,083</v>
+        <v>2,699,580</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>6/13/2020</v>
+        <v>6/14/2020</v>
       </c>
       <c r="B193" t="str">
-        <v>437,119</v>
+        <v>544,046</v>
       </c>
       <c r="C193" t="str">
-        <v>2,318,946</v>
+        <v>2,642,083</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>6/12/2020</v>
+        <v>6/13/2020</v>
       </c>
       <c r="B194" t="str">
-        <v>519,304</v>
+        <v>437,119</v>
       </c>
       <c r="C194" t="str">
-        <v>2,727,860</v>
+        <v>2,318,946</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>6/11/2020</v>
+        <v>6/12/2020</v>
       </c>
       <c r="B195" t="str">
-        <v>502,209</v>
+        <v>519,304</v>
       </c>
       <c r="C195" t="str">
-        <v>2,675,686</v>
+        <v>2,727,860</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>6/10/2020</v>
+        <v>6/11/2020</v>
       </c>
       <c r="B196" t="str">
-        <v>386,969</v>
+        <v>502,209</v>
       </c>
       <c r="C196" t="str">
-        <v>2,509,058</v>
+        <v>2,675,686</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>6/9/2020</v>
+        <v>6/10/2020</v>
       </c>
       <c r="B197" t="str">
-        <v>338,382</v>
+        <v>386,969</v>
       </c>
       <c r="C197" t="str">
-        <v>2,433,189</v>
+        <v>2,509,058</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>6/8/2020</v>
+        <v>6/9/2020</v>
       </c>
       <c r="B198" t="str">
-        <v>430,414</v>
+        <v>338,382</v>
       </c>
       <c r="C198" t="str">
-        <v>2,644,981</v>
+        <v>2,433,189</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>6/7/2020</v>
+        <v>6/8/2020</v>
       </c>
       <c r="B199" t="str">
-        <v>441,255</v>
+        <v>430,414</v>
       </c>
       <c r="C199" t="str">
-        <v>2,669,860</v>
+        <v>2,644,981</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>6/6/2020</v>
+        <v>6/7/2020</v>
       </c>
       <c r="B200" t="str">
-        <v>353,016</v>
+        <v>441,255</v>
       </c>
       <c r="C200" t="str">
-        <v>2,225,952</v>
+        <v>2,669,860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>